<commit_message>
tout a été refait
</commit_message>
<xml_diff>
--- a/Blocs.xlsx
+++ b/Blocs.xlsx
@@ -5,34 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\Diagonal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9EEAE37-9765-4B96-A209-643C52D9C9B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C7045A-2533-4F8F-B76E-66FB2AEE5573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17130" yWindow="4455" windowWidth="21600" windowHeight="11385" xr2:uid="{69FB41F2-F597-4267-A367-FA489D05BAE7}"/>
+    <workbookView xWindow="19920" yWindow="3600" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Numero</t>
   </si>
@@ -43,62 +36,144 @@
     <t>Collision</t>
   </si>
   <si>
+    <t>Utilisation</t>
+  </si>
+  <si>
+    <t>Vide</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Personnage</t>
+  </si>
+  <si>
+    <t>─</t>
+  </si>
+  <si>
+    <t>Barre Horizontale</t>
+  </si>
+  <si>
     <t>│</t>
   </si>
   <si>
-    <t>─</t>
+    <t>Barre Verticale</t>
   </si>
   <si>
     <t>┌</t>
   </si>
   <si>
+    <t>Coin</t>
+  </si>
+  <si>
     <t>┐</t>
   </si>
   <si>
+    <t>└</t>
+  </si>
+  <si>
     <t>┘</t>
   </si>
   <si>
-    <t>└</t>
-  </si>
-  <si>
-    <t>Utilisation</t>
-  </si>
-  <si>
-    <t>Coin</t>
-  </si>
-  <si>
-    <t>Barre Verticale</t>
-  </si>
-  <si>
-    <t>Barre Horizontale</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>Personnage</t>
-  </si>
-  <si>
-    <t>Vide</t>
+    <t>tete haut droit</t>
+  </si>
+  <si>
+    <t>tete bas droite</t>
+  </si>
+  <si>
+    <t>tet haut gauche</t>
+  </si>
+  <si>
+    <t>tete bas gauche</t>
+  </si>
+  <si>
+    <t>corps haut/droite → bas/droite</t>
+  </si>
+  <si>
+    <t>corps bas droite → haut droite</t>
+  </si>
+  <si>
+    <t>haut gauche *2</t>
+  </si>
+  <si>
+    <t>bas droite *2</t>
+  </si>
+  <si>
+    <t>bas droite → bas gauche</t>
+  </si>
+  <si>
+    <t>haut gauche → haut droite</t>
+  </si>
+  <si>
+    <t>╱</t>
+  </si>
+  <si>
+    <t>╲</t>
+  </si>
+  <si>
+    <t>˅</t>
+  </si>
+  <si>
+    <t>˄</t>
+  </si>
+  <si>
+    <t>˃</t>
+  </si>
+  <si>
+    <t>˂</t>
+  </si>
+  <si>
+    <t>⇗</t>
+  </si>
+  <si>
+    <t>⇘</t>
+  </si>
+  <si>
+    <t>⇙</t>
+  </si>
+  <si>
+    <t>⇖</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF202122"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF111111"/>
+      <name val="U0000"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF111111"/>
+      <name val="U2000"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF81787F"/>
+      <name val="U2000"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,15 +196,87 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF202122"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -437,19 +584,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAACFB-71F2-4A3E-9035-CFB0EEB40C54}">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="1025" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,10 +611,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -471,130 +622,255 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="23.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="23.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="23.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="23.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="23.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="23.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="23.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="23.25">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" ht="18">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18">
+      <c r="A13">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="23.25">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B16" s="1"/>
+    <row r="16" spans="1:4" ht="18">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="23.25">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="23.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18">
+      <c r="A22">
+        <v>16</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18">
+      <c r="A23">
+        <v>17</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout du niveau 1
</commit_message>
<xml_diff>
--- a/Blocs.xlsx
+++ b/Blocs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\Diagonal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E548637-CAB9-4136-82FF-FA2E44F55EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CE70E9-372C-4DE5-84CE-5365C28FA29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3600" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Numero</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>|</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Bloc</t>
   </si>
 </sst>
 </file>
@@ -568,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -852,6 +858,20 @@
         <v>18</v>
       </c>
     </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>